<commit_message>
Mais simulações e resultados
</commit_message>
<xml_diff>
--- a/tests/results/resultsSummary.xlsx
+++ b/tests/results/resultsSummary.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Date 1</t>
   </si>
@@ -81,12 +81,24 @@
   </si>
   <si>
     <t>Open log</t>
+  </si>
+  <si>
+    <t>All time</t>
+  </si>
+  <si>
+    <t>00003</t>
+  </si>
+  <si>
+    <t>Very strong ascending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +142,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -145,7 +169,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,8 +201,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -465,7 +498,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,43 +516,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -570,7 +603,87 @@
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="8"/>
+      <c r="B3" s="3">
+        <v>42964</v>
+      </c>
+      <c r="C3" s="3">
+        <v>43184</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2">
+        <v>55</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="4">
+        <v>2.4998</v>
+      </c>
+      <c r="L3" s="5">
+        <f>8000/4230-1</f>
+        <v>0.89125295508274238</v>
+      </c>
+      <c r="M3" s="9" t="str">
+        <f ca="1">HYPERLINK(CONCATENATE(LEFT(CELL("nome.arquivo"),SEARCH("[",CELL("nome.arquivo"))-1),"id",A3,".txt"),CONCATENATE("Open log id ",A3))</f>
+        <v>Open log id 00002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43086</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2">
+        <v>21</v>
+      </c>
+      <c r="I4" s="2">
+        <v>55</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.8165</v>
+      </c>
+      <c r="L4" s="14">
+        <f>20000/6400-1</f>
+        <v>2.125</v>
+      </c>
+      <c r="M4" s="9" t="str">
+        <f ca="1">HYPERLINK(CONCATENATE(LEFT(CELL("nome.arquivo"),SEARCH("[",CELL("nome.arquivo"))-1),"id",A4,".txt"),CONCATENATE("Open log id ",A4))</f>
+        <v>Open log id 00003</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M6" s="10"/>

</xml_diff>

<commit_message>
Limits da EMA como argumento da função de teste
</commit_message>
<xml_diff>
--- a/tests/results/resultsSummary.xlsx
+++ b/tests/results/resultsSummary.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Date 1</t>
   </si>
@@ -102,16 +102,23 @@
   </si>
   <si>
     <t>Ascending</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Rentability (day)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +137,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -187,7 +202,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,25 +231,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -519,11 +543,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -536,51 +558,59 @@
     <col min="11" max="11" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.85546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="14" width="10.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="17" t="s">
         <v>17</v>
       </c>
+      <c r="N1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -622,8 +652,16 @@
         <f ca="1">HYPERLINK(CONCATENATE(LEFT(CELL("nome.arquivo"),SEARCH("[",CELL("nome.arquivo"))-1),"id",A2,".txt"),CONCATENATE("Open log id ",A2))</f>
         <v>Open log id 00001</v>
       </c>
+      <c r="N2" s="1">
+        <f>C2-B2</f>
+        <v>51</v>
+      </c>
+      <c r="O2" s="19">
+        <f>(1+K2)^(1/N2)-1</f>
+        <v>-5.5678346345212626E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -633,7 +671,7 @@
       <c r="C3" s="2">
         <v>43184</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -665,8 +703,16 @@
         <f ca="1">HYPERLINK(CONCATENATE(LEFT(CELL("nome.arquivo"),SEARCH("[",CELL("nome.arquivo"))-1),"id",A3,".txt"),CONCATENATE("Open log id ",A3))</f>
         <v>Open log id 00002</v>
       </c>
+      <c r="N3" s="1">
+        <f t="shared" ref="N3:N6" si="0">C3-B3</f>
+        <v>220</v>
+      </c>
+      <c r="O3" s="19">
+        <f t="shared" ref="O3:O6" si="1">(1+K3)^(1/N3)-1</f>
+        <v>5.7103596821097558E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -700,7 +746,7 @@
       <c r="K4" s="3">
         <v>0.8165</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="10">
         <f>20000/6400-1</f>
         <v>2.125</v>
       </c>
@@ -708,8 +754,16 @@
         <f ca="1">HYPERLINK(CONCATENATE(LEFT(CELL("nome.arquivo"),SEARCH("[",CELL("nome.arquivo"))-1),"id",A4,".txt"),CONCATENATE("Open log id ",A4))</f>
         <v>Open log id 00003</v>
       </c>
+      <c r="N4" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="O4" s="19">
+        <f t="shared" si="1"/>
+        <v>1.7711239042295768E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
@@ -719,7 +773,7 @@
       <c r="C5" s="2">
         <v>43014</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -743,25 +797,33 @@
       <c r="K5" s="3">
         <v>9.5899999999999999E-2</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="13">
         <v>0</v>
       </c>
       <c r="M5" s="8" t="str">
         <f ca="1">HYPERLINK(CONCATENATE(LEFT(CELL("nome.arquivo"),SEARCH("[",CELL("nome.arquivo"))-1),"id",A5,".txt"),CONCATENATE("Open log id ",A5))</f>
         <v>Open log id 00004</v>
       </c>
+      <c r="N5" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="O5" s="19">
+        <f t="shared" si="1"/>
+        <v>1.833197124858188E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="2">
-        <v>43014</v>
+        <v>43013</v>
       </c>
       <c r="C6" s="2">
         <v>43052</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -783,7 +845,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="3">
-        <v>0.19639999999999999</v>
+        <v>0.58689999999999998</v>
       </c>
       <c r="L6" s="4">
         <f>6600/4300-1</f>
@@ -793,16 +855,24 @@
         <f ca="1">HYPERLINK(CONCATENATE(LEFT(CELL("nome.arquivo"),SEARCH("[",CELL("nome.arquivo"))-1),"id",A6,".txt"),CONCATENATE("Open log id ",A6))</f>
         <v>Open log id 00005</v>
       </c>
+      <c r="N6" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="O6" s="19">
+        <f t="shared" si="1"/>
+        <v>1.1910952169438271E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M7" s="7"/>
     </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N16" s="15"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M1">
-    <sortState ref="A2:M6">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:O1"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>